<commit_message>
updating manuscript and figures with pairwise comparison letters.
</commit_message>
<xml_diff>
--- a/Writing/Supplementary_Materials/Final Supp Materials April 22/Supplementary Tables.xlsx
+++ b/Writing/Supplementary_Materials/Final Supp Materials April 22/Supplementary Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gordoncuster/Desktop/Git_Projects/Herbicide_Microbes_PT1/Writing/Supplementary_Materials/Final Supp Materials April 22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E2DDF-0445-A14F-88F5-904B8EDE034B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F0F46-E433-B447-AF00-F3DA8D51EE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22260" yWindow="500" windowWidth="34380" windowHeight="27360" firstSheet="4" activeTab="11" xr2:uid="{3B2777A9-9730-A043-8EAE-74AD230F66E7}"/>
+    <workbookView xWindow="18140" yWindow="500" windowWidth="34380" windowHeight="27360" firstSheet="4" activeTab="11" xr2:uid="{3B2777A9-9730-A043-8EAE-74AD230F66E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Table legends" sheetId="10" r:id="rId1"/>
@@ -17782,6 +17782,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">

</xml_diff>